<commit_message>
Fixed output parsing logic not working with color code escape characters
</commit_message>
<xml_diff>
--- a/test_files/complex_cases.xlsx
+++ b/test_files/complex_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brt.hawayda\Desktop\42\minishell-jnde\minishell-tester\test_files\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640176BC-59C6-41FB-9D8D-31ED83C2F644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC6F648-A231-48D4-9391-90B0FC93B035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>$&gt; echo 'Hello World' | grep Hello | .wc -w &gt;&gt; output.txt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>$&gt; echo "         " | cat -e</t>
   </si>
   <si>
     <t>$&gt; echo -n "         " | cat -e</t>
+  </si>
+  <si>
+    <t>$&gt; echo $HOME
+hola</t>
+  </si>
+  <si>
+    <t>$&gt; echo $HOME
+$&gt; echo $HOME
+$&gt; echo $HOME</t>
+  </si>
+  <si>
+    <t>$&gt; echo $HOME
+$&gt; hola</t>
+  </si>
+  <si>
+    <t>$&gt; echo $HOME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+echo $HOME
+echo $HOME
+echo $HOME</t>
+  </si>
+  <si>
+    <t>$&gt; 
+$&gt; echo $HOME
+$&gt; echo $HOME
+$&gt; echo $HOME</t>
+  </si>
+  <si>
+    <t>echo $HOME
+echo $HOME
+echo $HOME</t>
   </si>
 </sst>
 </file>
@@ -69,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,13 +459,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>